<commit_message>
added filtering on assetid upon clicking on the overview
</commit_message>
<xml_diff>
--- a/data/Gemeente Almere bruggen components dummy.xlsx
+++ b/data/Gemeente Almere bruggen components dummy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia.paranich\Dropbox\MSc\DSP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Julia\GIT\DSP-B1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6645426-0614-4D64-ACC8-271BBFF4437C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD0636C-DDF0-498D-83D4-4F51FB918969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
   <si>
     <t>Assetnumber</t>
   </si>
@@ -37,9 +37,6 @@
     <t>ComponentVolume</t>
   </si>
   <si>
-    <t>ComponentNumber</t>
-  </si>
-  <si>
     <t>ComponentState</t>
   </si>
   <si>
@@ -62,6 +59,21 @@
   </si>
   <si>
     <t>Aluminum</t>
+  </si>
+  <si>
+    <t>ComponentAmount</t>
+  </si>
+  <si>
+    <t>Bolt</t>
+  </si>
+  <si>
+    <t>ComponentType</t>
+  </si>
+  <si>
+    <t>M24</t>
+  </si>
+  <si>
+    <t>ProductCode</t>
   </si>
 </sst>
 </file>
@@ -906,50 +918,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="38.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -960,7 +978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -968,10 +986,10 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -979,10 +997,10 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -990,10 +1008,10 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -1001,10 +1019,10 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -1015,7 +1033,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2275</v>
       </c>
@@ -1023,10 +1041,10 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2292</v>
       </c>
@@ -1037,7 +1055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>2293</v>
       </c>
@@ -1048,7 +1066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>2294</v>
       </c>
@@ -1056,10 +1074,10 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2502</v>
       </c>
@@ -1067,10 +1085,10 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>2503</v>
       </c>
@@ -1081,7 +1099,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2504</v>
       </c>
@@ -1089,10 +1107,10 @@
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2526</v>
       </c>
@@ -1100,10 +1118,10 @@
         <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>2527</v>
       </c>
@@ -1111,10 +1129,10 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>2528</v>
       </c>
@@ -1122,10 +1140,10 @@
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>2530</v>
       </c>
@@ -1136,7 +1154,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>2531</v>
       </c>
@@ -1147,7 +1165,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>2531</v>
       </c>
@@ -1158,7 +1176,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>2532</v>
       </c>
@@ -1169,7 +1187,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>3301</v>
       </c>
@@ -1177,10 +1195,10 @@
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>8005</v>
       </c>
@@ -1191,7 +1209,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>8008</v>
       </c>
@@ -1202,7 +1220,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>9038</v>
       </c>
@@ -1213,7 +1231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>3337</v>
       </c>
@@ -1224,7 +1242,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>3338</v>
       </c>
@@ -1235,7 +1253,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>3338</v>
       </c>
@@ -1243,7 +1261,21 @@
         <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>2293</v>
+      </c>
+      <c r="B29">
+        <v>10</v>
+      </c>
+      <c r="C29" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1256,6 +1288,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C88F1F5C68B5FB478F7E2F156521F34B" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="62ee8e2e48d66d65196d82c17f3e9601">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b668fa5a-6b34-45d2-a903-e7346e129eac" xmlns:ns3="d22ba816-bb7e-4df2-b860-2ad24d0868ea" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8d096f51100c27cbb5cfe357895179bc" ns2:_="" ns3:_="">
     <xsd:import namespace="b668fa5a-6b34-45d2-a903-e7346e129eac"/>
@@ -1478,15 +1519,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1494,6 +1526,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB808B59-242A-4ECE-A32E-F036B764A07E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0568FA5-61AF-43F2-83D2-40138979744D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1512,14 +1552,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB808B59-242A-4ECE-A32E-F036B764A07E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4E3BDDE-277E-4F6A-8A06-62E6AB4C2263}">
   <ds:schemaRefs>

</xml_diff>